<commit_message>
template folder for experiments
</commit_message>
<xml_diff>
--- a/ampl/experiments/sol/shock/output/gladlab-knitro-aus-agg.xlsx
+++ b/ampl/experiments/sol/shock/output/gladlab-knitro-aus-agg.xlsx
@@ -184,16 +184,16 @@
         <v>31.197412375203356</v>
       </c>
       <c r="D2" t="n">
-        <v>447.72675685895433</v>
+        <v>447.72675691069213</v>
       </c>
       <c r="E2" t="n">
-        <v>182.89167795308481</v>
+        <v>182.89167784199395</v>
       </c>
       <c r="F2" t="n">
-        <v>51.188111915488378</v>
+        <v>51.188111908216221</v>
       </c>
       <c r="G2" t="n">
-        <v>112.17212792491145</v>
+        <v>112.1721279456065</v>
       </c>
     </row>
     <row r="3">
@@ -204,19 +204,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>32.416364703580371</v>
+        <v>32.416364714563123</v>
       </c>
       <c r="D3" t="n">
-        <v>455.60011878286144</v>
+        <v>436.99235134094602</v>
       </c>
       <c r="E3" t="n">
-        <v>189.55223945569526</v>
+        <v>186.74848824692378</v>
       </c>
       <c r="F3" t="n">
-        <v>52.420757065688434</v>
+        <v>48.440894912266103</v>
       </c>
       <c r="G3" t="n">
-        <v>113.71689490008937</v>
+        <v>109.39897472307671</v>
       </c>
     </row>
     <row r="4">
@@ -227,19 +227,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>33.378544469982579</v>
+        <v>32.91097173227854</v>
       </c>
       <c r="D4" t="n">
-        <v>462.25562221464639</v>
+        <v>441.45440502531841</v>
       </c>
       <c r="E4" t="n">
-        <v>194.87702280996666</v>
+        <v>190.07425385812425</v>
       </c>
       <c r="F4" t="n">
-        <v>53.450217955247901</v>
+        <v>49.067314862631456</v>
       </c>
       <c r="G4" t="n">
-        <v>115.07100859114411</v>
+        <v>110.30597327572663</v>
       </c>
     </row>
     <row r="5">
@@ -250,19 +250,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>34.144699153279852</v>
+        <v>33.308083785147147</v>
       </c>
       <c r="D5" t="n">
-        <v>468.09468653631819</v>
+        <v>445.58723892673299</v>
       </c>
       <c r="E5" t="n">
-        <v>199.1255430236082</v>
+        <v>192.81465266787015</v>
       </c>
       <c r="F5" t="n">
-        <v>54.321607494283462</v>
+        <v>49.629281580298532</v>
       </c>
       <c r="G5" t="n">
-        <v>116.3054183110002</v>
+        <v>111.20019906705092</v>
       </c>
     </row>
     <row r="6">

</xml_diff>